<commit_message>
restructured for JS decision tree, example system.
</commit_message>
<xml_diff>
--- a/plantClinicData.xlsx
+++ b/plantClinicData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\OneDrive\Documents\Projects\plantDiagnostics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01592CF9-9CA3-47C4-A60E-D169317F7428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C705C1-D7AE-4850-A15A-94E8022FF720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2220" yWindow="5265" windowWidth="8310" windowHeight="11385" xr2:uid="{BC923BC4-1173-4E4C-BBF9-6E43D96E068D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC923BC4-1173-4E4C-BBF9-6E43D96E068D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="76">
   <si>
     <t>tropical</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>nasturtium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -613,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035B017E-37B4-4518-8C20-C568FF872E62}">
   <dimension ref="A1:Y121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +777,7 @@
         <v>9</v>
       </c>
       <c r="R4" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="S4" t="s">
         <v>11</v>
@@ -1212,7 +1215,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
@@ -1369,6 +1372,9 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
       </c>
       <c r="C40" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
added visual aspects of plant type selection feature
</commit_message>
<xml_diff>
--- a/plantClinicData.xlsx
+++ b/plantClinicData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\OneDrive\Documents\Projects\plantDiagnostics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C705C1-D7AE-4850-A15A-94E8022FF720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADA1ED3-4BF5-49FA-A174-C91C494E9D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC923BC4-1173-4E4C-BBF9-6E43D96E068D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="75">
   <si>
     <t>tropical</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>nasturtium</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -617,7 +614,7 @@
   <dimension ref="A1:Y121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +774,7 @@
         <v>9</v>
       </c>
       <c r="R4" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="S4" t="s">
         <v>11</v>

</xml_diff>